<commit_message>
Implement base export from mark accounting page
</commit_message>
<xml_diff>
--- a/web/templates/marks/exam.xlsx
+++ b/web/templates/marks/exam.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28315"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ЭтаКнига"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimka/Projects/arina/web/templates/marks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OSPanel\domains\arina\web\templates\marks\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6680" yWindow="460" windowWidth="22120" windowHeight="9780"/>
+    <workbookView xWindow="6675" yWindow="465" windowWidth="22125" windowHeight="9780"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -17,10 +17,10 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$1:$I$32</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -137,7 +137,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -216,7 +216,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -322,11 +322,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -349,7 +360,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -374,9 +384,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -384,6 +391,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -398,7 +408,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -416,18 +426,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -439,15 +437,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -801,67 +814,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Лист1" enableFormatConditionsCalculation="0">
+  <sheetPr codeName="Лист1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:T106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="5.1640625" customWidth="1"/>
-    <col min="3" max="3" width="4.5" customWidth="1"/>
-    <col min="4" max="4" width="29.5" customWidth="1"/>
-    <col min="5" max="5" width="5.33203125" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" customWidth="1"/>
-    <col min="8" max="8" width="6.33203125" customWidth="1"/>
-    <col min="9" max="9" width="29.1640625" customWidth="1"/>
+    <col min="1" max="2" width="5.140625" customWidth="1"/>
+    <col min="3" max="3" width="4.42578125" customWidth="1"/>
+    <col min="4" max="4" width="29.42578125" customWidth="1"/>
+    <col min="5" max="5" width="5.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" customWidth="1"/>
+    <col min="9" max="9" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-    </row>
-    <row r="2" spans="1:20" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+    </row>
+    <row r="2" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-    </row>
-    <row r="3" spans="1:20" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="43" t="s">
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+    </row>
+    <row r="3" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
@@ -870,13 +883,13 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="47" t="s">
+      <c r="G4" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
@@ -885,91 +898,91 @@
       <c r="D5" s="5"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="47" t="s">
+      <c r="G5" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
-      <c r="G6" s="47" t="s">
+      <c r="G6" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="47"/>
-      <c r="I6" s="47"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A7" s="46"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A8" s="30"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-    </row>
-    <row r="9" spans="1:20" ht="20" x14ac:dyDescent="0.2">
-      <c r="A9" s="44" t="s">
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A7" s="41"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A8" s="29"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+    </row>
+    <row r="9" spans="1:20" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A9" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="44"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A10" s="30"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-    </row>
-    <row r="11" spans="1:20" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="36" t="str">
+      <c r="B9" s="45"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A10" s="29"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+    </row>
+    <row r="11" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="35" t="str">
         <f>K101</f>
         <v>Предмет</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="36"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A12" s="45" t="s">
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A12" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="45"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="45"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
@@ -981,21 +994,21 @@
       <c r="S12" s="5"/>
       <c r="T12" s="5"/>
     </row>
-    <row r="13" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="6"/>
-      <c r="D13" s="36" t="str">
+      <c r="D13" s="35" t="str">
         <f>K102</f>
         <v>Спеціальність</v>
       </c>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="36"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
@@ -1007,24 +1020,24 @@
       <c r="S13" s="5"/>
       <c r="T13" s="5"/>
     </row>
-    <row r="14" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="40" t="str">
+      <c r="C14" s="39" t="str">
         <f>K103</f>
         <v>Семестр</v>
       </c>
-      <c r="D14" s="40"/>
+      <c r="D14" s="39"/>
       <c r="E14" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="41" t="str">
+      <c r="F14" s="46" t="str">
         <f>K104</f>
         <v>Курс</v>
       </c>
-      <c r="G14" s="41"/>
+      <c r="G14" s="46"/>
       <c r="H14" s="8" t="s">
         <v>20</v>
       </c>
@@ -1043,19 +1056,19 @@
       <c r="S14" s="5"/>
       <c r="T14" s="5"/>
     </row>
-    <row r="15" spans="1:20" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="36" t="str">
+    <row r="15" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="35" t="str">
         <f>K106</f>
         <v>Викладачі</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
@@ -1067,18 +1080,18 @@
       <c r="S15" s="5"/>
       <c r="T15" s="5"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A16" s="35" t="s">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A16" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
@@ -1090,16 +1103,16 @@
       <c r="S16" s="5"/>
       <c r="T16" s="5"/>
     </row>
-    <row r="17" spans="1:20" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
+    <row r="17" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="34"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
@@ -1111,23 +1124,23 @@
       <c r="S17" s="5"/>
       <c r="T17" s="5"/>
     </row>
-    <row r="18" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="24" t="s">
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="G18" s="37" t="s">
+      <c r="G18" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="H18" s="39"/>
+      <c r="H18" s="38"/>
       <c r="I18" s="10" t="s">
         <v>4</v>
       </c>
@@ -1142,16 +1155,16 @@
       <c r="S18" s="5"/>
       <c r="T18" s="5"/>
     </row>
-    <row r="19" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="13"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="12"/>
+    <row r="19" spans="1:20" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="27"/>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
@@ -1163,16 +1176,16 @@
       <c r="S19" s="5"/>
       <c r="T19" s="5"/>
     </row>
-    <row r="20" spans="1:20" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="15"/>
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="14"/>
+    <row r="20" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="13"/>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
@@ -1184,18 +1197,18 @@
       <c r="S20" s="5"/>
       <c r="T20" s="5"/>
     </row>
-    <row r="21" spans="1:20" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="16"/>
-      <c r="B21" s="33" t="s">
+    <row r="21" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="15"/>
+      <c r="B21" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="14"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="13"/>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>
@@ -1207,16 +1220,16 @@
       <c r="S21" s="5"/>
       <c r="T21" s="5"/>
     </row>
-    <row r="22" spans="1:20" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="16"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="28"/>
+    <row r="22" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="15"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="26"/>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
@@ -1228,12 +1241,12 @@
       <c r="S22" s="5"/>
       <c r="T22" s="5"/>
     </row>
-    <row r="23" spans="1:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="B23" s="18" t="s">
+    <row r="23" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B23" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
@@ -1245,17 +1258,17 @@
       <c r="S23" s="5"/>
       <c r="T23" s="5"/>
     </row>
-    <row r="24" spans="1:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="B24" s="23" t="s">
+    <row r="24" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B24" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="17"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="H24" s="19" t="s">
+      <c r="C24" s="16"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="H24" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="I24" s="21" t="s">
+      <c r="I24" s="20" t="s">
         <v>28</v>
       </c>
       <c r="K24" s="5"/>
@@ -1269,18 +1282,18 @@
       <c r="S24" s="5"/>
       <c r="T24" s="5"/>
     </row>
-    <row r="25" spans="1:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="B25" s="18" t="s">
+    <row r="25" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B25" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="17"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="H25" s="19" t="s">
+      <c r="C25" s="16"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="H25" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="I25" s="21" t="s">
+      <c r="I25" s="20" t="s">
         <v>28</v>
       </c>
       <c r="K25" s="5"/>
@@ -1294,14 +1307,14 @@
       <c r="S25" s="5"/>
       <c r="T25" s="5"/>
     </row>
-    <row r="26" spans="1:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="B26" s="18" t="s">
+    <row r="26" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B26" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="17"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
@@ -1313,14 +1326,14 @@
       <c r="S26" s="5"/>
       <c r="T26" s="5"/>
     </row>
-    <row r="27" spans="1:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="B27" s="18" t="s">
+    <row r="27" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B27" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="17"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
@@ -1332,14 +1345,14 @@
       <c r="S27" s="5"/>
       <c r="T27" s="5"/>
     </row>
-    <row r="28" spans="1:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="B28" s="18" t="s">
+    <row r="28" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B28" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="17"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
@@ -1351,11 +1364,11 @@
       <c r="S28" s="5"/>
       <c r="T28" s="5"/>
     </row>
-    <row r="29" spans="1:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="E29" s="20" t="s">
+    <row r="29" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="E29" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="F29" s="20"/>
+      <c r="F29" s="19"/>
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
       <c r="M29" s="5"/>
@@ -1367,7 +1380,7 @@
       <c r="S29" s="5"/>
       <c r="T29" s="5"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
       <c r="M30" s="5"/>
@@ -1379,70 +1392,67 @@
       <c r="S30" s="5"/>
       <c r="T30" s="5"/>
     </row>
-    <row r="31" spans="1:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="C31" s="23" t="s">
+    <row r="31" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C31" s="22" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="4"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
-    </row>
-    <row r="101" spans="11:11" x14ac:dyDescent="0.15">
+      <c r="G32" s="28"/>
+      <c r="H32" s="28"/>
+    </row>
+    <row r="101" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K101" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="102" spans="11:11" x14ac:dyDescent="0.15">
+    <row r="102" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K102" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="103" spans="11:11" x14ac:dyDescent="0.15">
+    <row r="103" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K103" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="104" spans="11:11" x14ac:dyDescent="0.15">
+    <row r="104" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K104" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="105" spans="11:11" x14ac:dyDescent="0.15">
+    <row r="105" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K105" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="106" spans="11:11" x14ac:dyDescent="0.15">
+    <row r="106" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K106" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A11:I11"/>
-    <mergeCell ref="A9:I9"/>
-    <mergeCell ref="A12:I12"/>
     <mergeCell ref="A7:H7"/>
     <mergeCell ref="G4:I4"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="G6:I6"/>
-    <mergeCell ref="D13:I13"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:I3"/>
     <mergeCell ref="A8:H8"/>
     <mergeCell ref="A15:I15"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="F14:G14"/>
+    <mergeCell ref="A12:I12"/>
+    <mergeCell ref="A11:I11"/>
+    <mergeCell ref="A9:I9"/>
     <mergeCell ref="G32:H32"/>
     <mergeCell ref="A10:H10"/>
     <mergeCell ref="B19:E19"/>
@@ -1453,6 +1463,9 @@
     <mergeCell ref="G21:H21"/>
     <mergeCell ref="A16:I16"/>
     <mergeCell ref="A17:I17"/>
+    <mergeCell ref="D13:I13"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="G18:H18"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>